<commit_message>
add pmas data and new experimentation
</commit_message>
<xml_diff>
--- a/Scripts/testing/var_weight_experiment_data.xlsx
+++ b/Scripts/testing/var_weight_experiment_data.xlsx
@@ -418,10 +418,13 @@
         <v>6.364408356086385</v>
       </c>
       <c r="F2">
-        <v>6.20762462462464</v>
+        <v>6.087478991596672</v>
+      </c>
+      <c r="G2">
+        <v>6.632064627284575</v>
       </c>
       <c r="H2">
-        <v>6.429775827962118</v>
+        <v>6.532849534453788</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -441,10 +444,13 @@
         <v>7.289915623465775</v>
       </c>
       <c r="F3">
-        <v>7.410894465894434</v>
+        <v>7.07791596638653</v>
+      </c>
+      <c r="G3">
+        <v>6.934768102664178</v>
       </c>
       <c r="H3">
-        <v>6.737994719848222</v>
+        <v>6.832509762093848</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -464,10 +470,13 @@
         <v>6.835476215496203</v>
       </c>
       <c r="F4">
-        <v>6.625362719862705</v>
+        <v>6.629642296918772</v>
+      </c>
+      <c r="G4">
+        <v>7.049883377082129</v>
       </c>
       <c r="H4">
-        <v>6.848968328882646</v>
+        <v>6.94990825857364</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -487,10 +496,13 @@
         <v>7.308803638905326</v>
       </c>
       <c r="F5">
-        <v>7.318629129129112</v>
+        <v>7.500521848739495</v>
+      </c>
+      <c r="G5">
+        <v>7.164795115113377</v>
       </c>
       <c r="H5">
-        <v>6.96644189406971</v>
+        <v>7.063406280703199</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -510,10 +522,13 @@
         <v>6.804318165134595</v>
       </c>
       <c r="F6">
-        <v>6.672957957957938</v>
+        <v>6.677237535014005</v>
+      </c>
+      <c r="G6">
+        <v>7.097467445262037</v>
       </c>
       <c r="H6">
-        <v>6.896361923902345</v>
+        <v>6.99759762443464</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -533,10 +548,13 @@
         <v>6.812200915866731</v>
       </c>
       <c r="F7">
-        <v>6.890250341250328</v>
+        <v>7.07214306086071</v>
+      </c>
+      <c r="G7">
+        <v>6.736394667201086</v>
       </c>
       <c r="H7">
-        <v>6.537670325260655</v>
+        <v>6.635210343247174</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -556,10 +574,13 @@
         <v>6.604342573237562</v>
       </c>
       <c r="F8">
-        <v>6.74552306852309</v>
+        <v>6.927415788133472</v>
+      </c>
+      <c r="G8">
+        <v>6.591638873269897</v>
       </c>
       <c r="H8">
-        <v>6.392426252869706</v>
+        <v>6.490723769041995</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -579,10 +600,13 @@
         <v>6.694133656632486</v>
       </c>
       <c r="F9">
-        <v>6.726701686301681</v>
+        <v>6.687184443007967</v>
+      </c>
+      <c r="G9">
+        <v>6.796180113582604</v>
       </c>
       <c r="H9">
-        <v>6.596297496115819</v>
+        <v>6.695634697635617</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -602,10 +626,13 @@
         <v>6.882831557132721</v>
       </c>
       <c r="F10">
-        <v>6.800597993597981</v>
+        <v>6.982490713208363</v>
+      </c>
+      <c r="G10">
+        <v>6.646765413225019</v>
       </c>
       <c r="H10">
-        <v>6.448436765336219</v>
+        <v>6.545363040921147</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -625,10 +652,13 @@
         <v>6.490260748749909</v>
       </c>
       <c r="F11">
-        <v>6.306386529386512</v>
+        <v>6.621971988795511</v>
+      </c>
+      <c r="G11">
+        <v>6.73093246143</v>
       </c>
       <c r="H11">
-        <v>6.5304486696365</v>
+        <v>6.630719031321313</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -648,10 +678,13 @@
         <v>6.982423411226502</v>
       </c>
       <c r="F12">
-        <v>7.009930180180167</v>
+        <v>6.676951680672263</v>
+      </c>
+      <c r="G12">
+        <v>6.533762090407221</v>
       </c>
       <c r="H12">
-        <v>6.336271863236729</v>
+        <v>6.431898067813862</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -671,10 +704,13 @@
         <v>6.681457847302357</v>
       </c>
       <c r="F13">
-        <v>6.661673405758705</v>
+        <v>6.622156162464992</v>
+      </c>
+      <c r="G13">
+        <v>6.731168164256895</v>
       </c>
       <c r="H13">
-        <v>6.531564718665587</v>
+        <v>6.630468669190537</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -694,10 +730,13 @@
         <v>6.632785411408595</v>
       </c>
       <c r="F14">
-        <v>6.624622752163944</v>
+        <v>6.585105508870231</v>
+      </c>
+      <c r="G14">
+        <v>6.694114806625117</v>
       </c>
       <c r="H14">
-        <v>6.494465126834295</v>
+        <v>6.593440825069703</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -717,10 +756,13 @@
         <v>6.975614139765609</v>
       </c>
       <c r="F15">
-        <v>7.109566145092434</v>
+        <v>7.00377532065456</v>
+      </c>
+      <c r="G15">
+        <v>6.633364304659977</v>
       </c>
       <c r="H15">
-        <v>6.435294963101637</v>
+        <v>6.531819100672684</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -740,10 +782,13 @@
         <v>6.351744455627695</v>
       </c>
       <c r="F16">
-        <v>6.43049925715188</v>
+        <v>6.390982013858166</v>
+      </c>
+      <c r="G16">
+        <v>6.499972782710001</v>
       </c>
       <c r="H16">
-        <v>6.300006402743366</v>
+        <v>6.399473607363614</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -763,10 +808,13 @@
         <v>6.678065205662575</v>
       </c>
       <c r="F17">
-        <v>6.568510081510061</v>
+        <v>6.750402801120443</v>
+      </c>
+      <c r="G17">
+        <v>6.4146698621414</v>
       </c>
       <c r="H17">
-        <v>6.21621029235765</v>
+        <v>6.313339622504748</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -786,10 +834,13 @@
         <v>6.248325690950894</v>
       </c>
       <c r="F18">
-        <v>6.361601786201774</v>
+        <v>6.322084542908061</v>
+      </c>
+      <c r="G18">
+        <v>6.431068045664651</v>
       </c>
       <c r="H18">
-        <v>6.230977524875404</v>
+        <v>6.330637410741721</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -809,10 +860,13 @@
         <v>6.150135243748897</v>
       </c>
       <c r="F19">
-        <v>6.2201054564446</v>
+        <v>6.180588213150886</v>
+      </c>
+      <c r="G19">
+        <v>6.289582612757311</v>
       </c>
       <c r="H19">
-        <v>6.089678275200469</v>
+        <v>6.189049186779274</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -832,10 +886,13 @@
         <v>6.469118024212042</v>
       </c>
       <c r="F20">
-        <v>6.371889998694305</v>
+        <v>6.553782718304688</v>
+      </c>
+      <c r="G20">
+        <v>6.2180432363297</v>
       </c>
       <c r="H20">
-        <v>6.019471554531385</v>
+        <v>6.116774775479422</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -855,10 +912,13 @@
         <v>5.817703874386671</v>
       </c>
       <c r="F21">
-        <v>5.710391291291271</v>
+        <v>6.025976750700269</v>
+      </c>
+      <c r="G21">
+        <v>6.134936842972269</v>
       </c>
       <c r="H21">
-        <v>5.934446558487236</v>
+        <v>6.034726999725964</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -878,10 +938,13 @@
         <v>5.630070943373396</v>
       </c>
       <c r="F22">
-        <v>5.565706675906665</v>
+        <v>5.881292135315664</v>
+      </c>
+      <c r="G22">
+        <v>5.990245273527879</v>
       </c>
       <c r="H22">
-        <v>5.789636299456349</v>
+        <v>5.890101005207271</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -901,10 +964,13 @@
         <v>5.349165536106939</v>
       </c>
       <c r="F23">
-        <v>5.494091861091843</v>
+        <v>5.498371438147911</v>
+      </c>
+      <c r="G23">
+        <v>5.918590897439366</v>
       </c>
       <c r="H23">
-        <v>5.717307227124119</v>
+        <v>5.818819584832688</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -924,10 +990,13 @@
         <v>5.380482396643576</v>
       </c>
       <c r="F24">
-        <v>5.560425740025735</v>
+        <v>5.520908496732022</v>
+      </c>
+      <c r="G24">
+        <v>5.629886308814923</v>
       </c>
       <c r="H24">
-        <v>5.42969858402893</v>
+        <v>5.529509349679705</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -947,10 +1016,13 @@
         <v>5.542694733401513</v>
       </c>
       <c r="F25">
-        <v>5.588854909096289</v>
+        <v>5.770747628706672</v>
+      </c>
+      <c r="G25">
+        <v>5.434974314537371</v>
       </c>
       <c r="H25">
-        <v>5.235823312260324</v>
+        <v>5.334025226916956</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -970,10 +1042,13 @@
         <v>4.564184424065443</v>
       </c>
       <c r="F26">
-        <v>4.915302785544168</v>
+        <v>4.7951571525162</v>
+      </c>
+      <c r="G26">
+        <v>5.339785756949938</v>
       </c>
       <c r="H26">
-        <v>5.138228361980805</v>
+        <v>5.240165846126454</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -993,10 +1068,13 @@
         <v>4.928619171185334</v>
       </c>
       <c r="F27">
-        <v>5.137006897219791</v>
+        <v>5.097489653926078</v>
+      </c>
+      <c r="G27">
+        <v>5.206463388227134</v>
       </c>
       <c r="H27">
-        <v>5.006206020968205</v>
+        <v>5.106124889630204</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1016,10 +1094,13 @@
         <v>4.141976586145732</v>
       </c>
       <c r="F28">
-        <v>4.625561452581604</v>
+        <v>4.505415819553637</v>
+      </c>
+      <c r="G28">
+        <v>5.050013822030307</v>
       </c>
       <c r="H28">
-        <v>4.847935419162155</v>
+        <v>4.950682239173527</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1039,10 +1120,13 @@
         <v>5.287535803096818</v>
       </c>
       <c r="F29">
-        <v>5.267907452907441</v>
+        <v>5.162116628469567</v>
+      </c>
+      <c r="G29">
+        <v>4.791717453407658</v>
       </c>
       <c r="H29">
-        <v>4.593851213545612</v>
+        <v>4.69006040949986</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1062,10 +1146,13 @@
         <v>5.008420740695399</v>
       </c>
       <c r="F30">
-        <v>4.907769057827869</v>
+        <v>5.089661777438251</v>
+      </c>
+      <c r="G30">
+        <v>4.753920103582146</v>
       </c>
       <c r="H30">
-        <v>4.555310870002366</v>
+        <v>4.65267233744249</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1085,10 +1172,13 @@
         <v>4.506957625538174</v>
       </c>
       <c r="F31">
-        <v>4.652839372145237</v>
+        <v>4.613322128851524</v>
+      </c>
+      <c r="G31">
+        <v>4.722303526162458</v>
       </c>
       <c r="H31">
-        <v>4.52217703953007</v>
+        <v>4.621892750695715</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1108,10 +1198,13 @@
         <v>3.997802380815504</v>
       </c>
       <c r="F32">
-        <v>4.203846846846841</v>
+        <v>4.083701213818873</v>
+      </c>
+      <c r="G32">
+        <v>4.628337326109993</v>
       </c>
       <c r="H32">
-        <v>4.426907836457835</v>
+        <v>4.52864666194311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added experiment 1 code
</commit_message>
<xml_diff>
--- a/Scripts/testing/var_weight_experiment_data.xlsx
+++ b/Scripts/testing/var_weight_experiment_data.xlsx
@@ -418,13 +418,10 @@
         <v>6.364408356086385</v>
       </c>
       <c r="F2">
-        <v>6.087478991596672</v>
-      </c>
-      <c r="G2">
-        <v>6.632064627284575</v>
+        <v>0.02023634318839907</v>
       </c>
       <c r="H2">
-        <v>6.532849534453788</v>
+        <v>-0.02915623868895263</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -444,13 +441,10 @@
         <v>7.289915623465775</v>
       </c>
       <c r="F3">
-        <v>7.07791596638653</v>
-      </c>
-      <c r="G3">
-        <v>6.934768102664178</v>
+        <v>0.1013168047700807</v>
       </c>
       <c r="H3">
-        <v>6.832509762093848</v>
+        <v>-0.03067237533543543</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -470,13 +464,10 @@
         <v>6.835476215496203</v>
       </c>
       <c r="F4">
-        <v>6.629642296918772</v>
-      </c>
-      <c r="G4">
-        <v>7.049883377082129</v>
+        <v>-0.2859040023064409</v>
       </c>
       <c r="H4">
-        <v>6.94990825857364</v>
+        <v>-0.03230520711213458</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -496,13 +487,10 @@
         <v>7.308803638905326</v>
       </c>
       <c r="F5">
-        <v>7.500521848739495</v>
-      </c>
-      <c r="G5">
-        <v>7.164795115113377</v>
+        <v>0.02023634318839907</v>
       </c>
       <c r="H5">
-        <v>7.063406280703199</v>
+        <v>-0.02930843720673171</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -522,13 +510,10 @@
         <v>6.804318165134595</v>
       </c>
       <c r="F6">
-        <v>6.677237535014005</v>
-      </c>
-      <c r="G6">
-        <v>7.097467445262037</v>
+        <v>-0.3767851726253837</v>
       </c>
       <c r="H6">
-        <v>6.99759762443464</v>
+        <v>-0.03145701400854761</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -548,13 +533,10 @@
         <v>6.812200915866731</v>
       </c>
       <c r="F7">
-        <v>7.07214306086071</v>
-      </c>
-      <c r="G7">
-        <v>6.736394667201086</v>
+        <v>-0.1162825941674294</v>
       </c>
       <c r="H7">
-        <v>6.635210343247174</v>
+        <v>-0.04068344190870687</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -574,13 +556,10 @@
         <v>6.604342573237562</v>
       </c>
       <c r="F8">
-        <v>6.927415788133472</v>
-      </c>
-      <c r="G8">
-        <v>6.591638873269897</v>
+        <v>0.1206427006000514</v>
       </c>
       <c r="H8">
-        <v>6.490723769041995</v>
+        <v>-0.03098559925908104</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -600,13 +579,10 @@
         <v>6.694133656632486</v>
       </c>
       <c r="F9">
-        <v>6.687184443007967</v>
-      </c>
-      <c r="G9">
-        <v>6.796180113582604</v>
+        <v>-0.3297628183503412</v>
       </c>
       <c r="H9">
-        <v>6.695634697635617</v>
+        <v>-0.04173023469976335</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -626,13 +602,10 @@
         <v>6.882831557132721</v>
       </c>
       <c r="F10">
-        <v>6.982490713208363</v>
-      </c>
-      <c r="G10">
-        <v>6.646765413225019</v>
+        <v>0.01233230957495361</v>
       </c>
       <c r="H10">
-        <v>6.545363040921147</v>
+        <v>-0.04013200448336178</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -652,13 +625,10 @@
         <v>6.490260748749909</v>
       </c>
       <c r="F11">
-        <v>6.621971988795511</v>
-      </c>
-      <c r="G11">
-        <v>6.73093246143</v>
+        <v>-0.3556198415185821</v>
       </c>
       <c r="H11">
-        <v>6.630719031321313</v>
+        <v>-0.04783913451522626</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -678,13 +648,10 @@
         <v>6.982423411226502</v>
       </c>
       <c r="F12">
-        <v>6.676951680672263</v>
-      </c>
-      <c r="G12">
-        <v>6.533762090407221</v>
+        <v>0.132025025699478</v>
       </c>
       <c r="H12">
-        <v>6.431898067813862</v>
+        <v>-0.04586944825788503</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -704,13 +671,10 @@
         <v>6.681457847302357</v>
       </c>
       <c r="F13">
-        <v>6.622156162464992</v>
-      </c>
-      <c r="G13">
-        <v>6.731168164256895</v>
+        <v>-0.2343712103023051</v>
       </c>
       <c r="H13">
-        <v>6.630468669190537</v>
+        <v>-0.04721801424869909</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -730,13 +694,10 @@
         <v>6.632785411408595</v>
       </c>
       <c r="F14">
-        <v>6.585105508870231</v>
-      </c>
-      <c r="G14">
-        <v>6.694114806625117</v>
+        <v>0.1972432691056193</v>
       </c>
       <c r="H14">
-        <v>6.593440825069703</v>
+        <v>-0.05046050730132924</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -756,13 +717,10 @@
         <v>6.975614139765609</v>
       </c>
       <c r="F15">
-        <v>7.00377532065456</v>
-      </c>
-      <c r="G15">
-        <v>6.633364304659977</v>
+        <v>0.2956122349779051</v>
       </c>
       <c r="H15">
-        <v>6.531819100672684</v>
+        <v>-0.05410925584232507</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -782,13 +740,10 @@
         <v>6.351744455627695</v>
       </c>
       <c r="F16">
-        <v>6.390982013858166</v>
-      </c>
-      <c r="G16">
-        <v>6.499972782710001</v>
+        <v>-0.21175444599907</v>
       </c>
       <c r="H16">
-        <v>6.399473607363614</v>
+        <v>-0.05860944282376654</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -808,13 +763,10 @@
         <v>6.678065205662575</v>
       </c>
       <c r="F17">
-        <v>6.750402801120443</v>
-      </c>
-      <c r="G17">
-        <v>6.4146698621414</v>
+        <v>0.08280792306821345</v>
       </c>
       <c r="H17">
-        <v>6.313339622504748</v>
+        <v>-0.05676506090363112</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -834,13 +786,10 @@
         <v>6.248325690950894</v>
       </c>
       <c r="F18">
-        <v>6.322084542908061</v>
-      </c>
-      <c r="G18">
-        <v>6.431068045664651</v>
+        <v>-0.2007598915012807</v>
       </c>
       <c r="H18">
-        <v>6.330637410741721</v>
+        <v>-0.05438311111253059</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -860,13 +809,10 @@
         <v>6.150135243748897</v>
       </c>
       <c r="F19">
-        <v>6.180588213150886</v>
-      </c>
-      <c r="G19">
-        <v>6.289582612757311</v>
+        <v>0.06140240701563842</v>
       </c>
       <c r="H19">
-        <v>6.189049186779274</v>
+        <v>-0.05908256685437385</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -886,13 +832,10 @@
         <v>6.469118024212042</v>
       </c>
       <c r="F20">
-        <v>6.553782718304688</v>
-      </c>
-      <c r="G20">
-        <v>6.2180432363297</v>
+        <v>0.06140240701563842</v>
       </c>
       <c r="H20">
-        <v>6.116774775479422</v>
+        <v>-0.06373444709153075</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -912,13 +855,10 @@
         <v>5.817703874386671</v>
       </c>
       <c r="F21">
-        <v>6.025976750700269</v>
-      </c>
-      <c r="G21">
-        <v>6.134936842972269</v>
+        <v>-0.2915000674038085</v>
       </c>
       <c r="H21">
-        <v>6.034726999725964</v>
+        <v>-0.06919671797134891</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -938,13 +878,10 @@
         <v>5.630070943373396</v>
       </c>
       <c r="F22">
-        <v>5.881292135315664</v>
-      </c>
-      <c r="G22">
-        <v>5.990245273527879</v>
+        <v>-0.4538669545145184</v>
       </c>
       <c r="H22">
-        <v>5.890101005207271</v>
+        <v>-0.07166554474747217</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -964,13 +901,10 @@
         <v>5.349165536106939</v>
       </c>
       <c r="F23">
-        <v>5.498371438147911</v>
-      </c>
-      <c r="G23">
-        <v>5.918590897439366</v>
+        <v>-0.4538669545145184</v>
       </c>
       <c r="H23">
-        <v>5.818819584832688</v>
+        <v>-0.07376537875540018</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -990,13 +924,10 @@
         <v>5.380482396643576</v>
       </c>
       <c r="F24">
-        <v>5.520908496732022</v>
-      </c>
-      <c r="G24">
-        <v>5.629886308814923</v>
+        <v>-0.318272682631718</v>
       </c>
       <c r="H24">
-        <v>5.529509349679705</v>
+        <v>-0.06839602971398098</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1016,13 +947,10 @@
         <v>5.542694733401513</v>
       </c>
       <c r="F25">
-        <v>5.770747628706672</v>
-      </c>
-      <c r="G25">
-        <v>5.434974314537371</v>
+        <v>-0.009077992029759957</v>
       </c>
       <c r="H25">
-        <v>5.334025226916956</v>
+        <v>-0.07383933164862536</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1042,13 +970,10 @@
         <v>4.564184424065443</v>
       </c>
       <c r="F26">
-        <v>4.7951571525162</v>
-      </c>
-      <c r="G26">
-        <v>5.339785756949938</v>
+        <v>-0.4538669545145184</v>
       </c>
       <c r="H26">
-        <v>5.240165846126454</v>
+        <v>-0.09768858188808835</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1068,13 +993,10 @@
         <v>4.928619171185334</v>
       </c>
       <c r="F27">
-        <v>5.097489653926078</v>
-      </c>
-      <c r="G27">
-        <v>5.206463388227134</v>
+        <v>-0.3505111980378801</v>
       </c>
       <c r="H27">
-        <v>5.106124889630204</v>
+        <v>-0.1015155303933532</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1094,13 +1016,10 @@
         <v>4.141976586145732</v>
       </c>
       <c r="F28">
-        <v>4.505415819553637</v>
-      </c>
-      <c r="G28">
-        <v>5.050013822030307</v>
+        <v>-0.4538669545145184</v>
       </c>
       <c r="H28">
-        <v>4.950682239173527</v>
+        <v>-0.09970411375571463</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1120,13 +1039,10 @@
         <v>5.287535803096818</v>
       </c>
       <c r="F29">
-        <v>5.162116628469567</v>
-      </c>
-      <c r="G29">
-        <v>4.791717453407658</v>
+        <v>0.1987729760015876</v>
       </c>
       <c r="H29">
-        <v>4.69006040949986</v>
+        <v>-0.09642294950427645</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1146,13 +1062,10 @@
         <v>5.008420740695399</v>
       </c>
       <c r="F30">
-        <v>5.089661777438251</v>
-      </c>
-      <c r="G30">
-        <v>4.753920103582146</v>
+        <v>0.1281187015163463</v>
       </c>
       <c r="H30">
-        <v>4.65267233744249</v>
+        <v>-0.07080499003679154</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1172,13 +1085,10 @@
         <v>4.506957625538174</v>
       </c>
       <c r="F31">
-        <v>4.613322128851524</v>
-      </c>
-      <c r="G31">
-        <v>4.722303526162458</v>
+        <v>-0.03048350808233497</v>
       </c>
       <c r="H31">
-        <v>4.621892750695715</v>
+        <v>-0.07984220631471847</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1198,13 +1108,10 @@
         <v>3.997802380815504</v>
       </c>
       <c r="F32">
-        <v>4.083701213818873</v>
-      </c>
-      <c r="G32">
-        <v>4.628337326109993</v>
+        <v>-0.4538669545145184</v>
       </c>
       <c r="H32">
-        <v>4.52864666194311</v>
+        <v>-0.08839472913129356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>